<commit_message>
Preparing the module for updating the driving school
Module updates and preparation for further implementation of obtaining rights! also added school interior
</commit_message>
<xml_diff>
--- a/dotnet/resources/Информация.xlsx
+++ b/dotnet/resources/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Команда</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>fakeipl</t>
+  </si>
+  <si>
+    <t>veh</t>
+  </si>
+  <si>
+    <t>givelic</t>
+  </si>
+  <si>
+    <t>newrentveh</t>
+  </si>
+  <si>
+    <t>Выдача гос лицензий</t>
+  </si>
+  <si>
+    <t>Создания арендуемого автомобиля</t>
+  </si>
+  <si>
+    <t>Заспамить транспорт</t>
   </si>
 </sst>
 </file>
@@ -554,7 +572,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,23 +766,35 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
The second blank for the module of delivery of rights! It's not over yet
</commit_message>
<xml_diff>
--- a/dotnet/resources/Информация.xlsx
+++ b/dotnet/resources/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Команда</t>
   </si>
@@ -45,15 +45,6 @@
     <t>Выдать донат валюту</t>
   </si>
   <si>
-    <t>Фикс</t>
-  </si>
-  <si>
-    <t>Да</t>
-  </si>
-  <si>
-    <t>Нет</t>
-  </si>
-  <si>
     <t>createbusiness</t>
   </si>
   <si>
@@ -127,6 +118,15 @@
   </si>
   <si>
     <t>Заспамить транспорт</t>
+  </si>
+  <si>
+    <t>newjobveh</t>
+  </si>
+  <si>
+    <t>Заспамить транспорт для работы</t>
+  </si>
+  <si>
+    <t>[name] [model] [number] [c1] [c2]</t>
   </si>
 </sst>
 </file>
@@ -207,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,13 +230,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -273,9 +286,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -284,8 +294,33 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -572,20 +607,20 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -596,339 +631,327 @@
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="D4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="4"/>
+      <c r="D17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="25"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="4"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="25"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="4"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>